<commit_message>
(hotfix)record messages into Excel file
</commit_message>
<xml_diff>
--- a/messenger/messages.xlsx
+++ b/messenger/messages.xlsx
@@ -2,22 +2,22 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Messages" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="yyyy-mm-dd h:mm:ss"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -48,13 +48,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -419,14 +418,11 @@
   </sheetPr>
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="18.28515625" bestFit="1" customWidth="1" min="1" max="1"/>
-  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -452,7 +448,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>45051.61453230324</v>
+        <v>45051.61481586432</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -466,13 +462,13 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Zgxfncmv,hbjnk.m</t>
+          <t>gzhxcjvkbnjmjob.v,gcmfdxncmv,bh</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="n">
-        <v>45051.61481586432</v>
+      <c r="A3" s="1" t="n">
+        <v>45051.61453230146</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -486,7 +482,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>gzhxcjvkbnjmjob.v,gcmfdxncmv,bh</t>
+          <t>Zgxfncmv,hbjnk.m</t>
         </is>
       </c>
     </row>

</xml_diff>